<commit_message>
Median corrections and new summary
</commit_message>
<xml_diff>
--- a/results/GSVA_MEDIAN_summary.xlsx
+++ b/results/GSVA_MEDIAN_summary.xlsx
@@ -376,7 +376,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
@@ -386,7 +386,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>450</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>